<commit_message>
Run 4.2.R up to creating ps4 with data that incorporates manual Excel edits; add code section that removes duplicate observations of the same species in both subplot and 2x2 data for present_species table
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/04.2b_edited1_SpeciesSeeded-in-mix-assigned.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/04.2b_edited1_SpeciesSeeded-in-mix-assigned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="13_ncr:40009_{4E2DAE92-AEF9-46BE-997C-3D03E1D04585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47235C7C-9564-4A21-9D27-F6684953C5F0}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="13_ncr:40009_{4E2DAE92-AEF9-46BE-997C-3D03E1D04585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0537AF8D-EAF5-4125-AB91-A7BD7C04FFFF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="167">
   <si>
     <t>Region</t>
   </si>
@@ -1097,7 +1097,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>196215</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>131445</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1323,6 +1323,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1622,11 +1626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A203" sqref="A203:XFD213"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1938,7 +1942,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1949,16 +1953,16 @@
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1969,16 +1973,16 @@
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>163</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>163</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>122</v>
@@ -1992,19 +1996,19 @@
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>104</v>
+        <v>164</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2015,16 +2019,16 @@
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>104</v>
@@ -2038,16 +2042,16 @@
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>104</v>
@@ -2058,19 +2062,19 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>104</v>
@@ -2084,19 +2088,19 @@
         <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2110,13 +2114,13 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>122</v>
@@ -2130,16 +2134,16 @@
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>122</v>
@@ -2156,13 +2160,13 @@
         <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>122</v>
@@ -2170,22 +2174,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>122</v>
@@ -2202,7 +2206,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>36</v>
@@ -2225,7 +2229,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>36</v>
@@ -2248,7 +2252,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>36</v>
@@ -2271,7 +2275,7 @@
         <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>36</v>
@@ -2294,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>36</v>
@@ -2317,7 +2321,7 @@
         <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>36</v>
@@ -2340,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>36</v>
@@ -2363,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>36</v>
@@ -2386,7 +2390,7 @@
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>36</v>
@@ -2409,7 +2413,7 @@
         <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>36</v>
@@ -2432,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>36</v>
@@ -2455,7 +2459,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>36</v>
@@ -2478,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>36</v>
@@ -2501,7 +2505,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>36</v>
@@ -2524,7 +2528,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>36</v>
@@ -2547,7 +2551,7 @@
         <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>36</v>
@@ -2559,7 +2563,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -2567,10 +2571,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>36</v>
@@ -2578,8 +2582,8 @@
       <c r="F41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>122</v>
+      <c r="G41" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2593,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>36</v>
@@ -2616,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>36</v>
@@ -2639,7 +2643,7 @@
         <v>7</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>36</v>
@@ -2662,7 +2666,7 @@
         <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>36</v>
@@ -2685,7 +2689,7 @@
         <v>7</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>36</v>
@@ -2708,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>36</v>
@@ -2731,7 +2735,7 @@
         <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>36</v>
@@ -2754,7 +2758,7 @@
         <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>36</v>
@@ -2777,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>36</v>
@@ -2800,7 +2804,7 @@
         <v>7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>36</v>
@@ -2823,7 +2827,7 @@
         <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>36</v>
@@ -2846,7 +2850,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>36</v>
@@ -2869,7 +2873,7 @@
         <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>36</v>
@@ -2892,7 +2896,7 @@
         <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>36</v>
@@ -2915,7 +2919,7 @@
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>36</v>
@@ -2938,7 +2942,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>126</v>
+        <v>63</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>36</v>
@@ -2961,7 +2965,7 @@
         <v>7</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>36</v>
@@ -2984,7 +2988,7 @@
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>36</v>
@@ -3007,7 +3011,7 @@
         <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>36</v>
@@ -3030,7 +3034,7 @@
         <v>7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>36</v>
@@ -3053,7 +3057,7 @@
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>36</v>
@@ -3076,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>36</v>
@@ -3099,7 +3103,7 @@
         <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>36</v>
@@ -3122,7 +3126,7 @@
         <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>36</v>
@@ -3145,7 +3149,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>36</v>
@@ -3168,7 +3172,7 @@
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>36</v>
@@ -3191,7 +3195,7 @@
         <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>36</v>
@@ -3214,13 +3218,13 @@
         <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>122</v>
@@ -3237,13 +3241,13 @@
         <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>122</v>
@@ -3260,13 +3264,13 @@
         <v>7</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>122</v>
@@ -3283,7 +3287,7 @@
         <v>7</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>10</v>
@@ -3306,7 +3310,7 @@
         <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>10</v>
@@ -3329,7 +3333,7 @@
         <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>10</v>
@@ -3342,22 +3346,22 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>29</v>
-      </c>
-      <c r="B75" t="s">
-        <v>30</v>
-      </c>
-      <c r="C75" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" t="s">
-        <v>56</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="A75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G75" s="3" t="s">
@@ -3375,7 +3379,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>10</v>
@@ -3388,22 +3392,22 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="A77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" t="s">
         <v>107</v>
       </c>
       <c r="G77" s="3" t="s">
@@ -3421,7 +3425,7 @@
         <v>7</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>10</v>
@@ -3444,7 +3448,7 @@
         <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>10</v>
@@ -3467,7 +3471,7 @@
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>10</v>
@@ -3490,7 +3494,7 @@
         <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>10</v>
@@ -3513,13 +3517,13 @@
         <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>122</v>
@@ -3536,13 +3540,13 @@
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>122</v>
@@ -3559,7 +3563,7 @@
         <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>64</v>
@@ -3582,7 +3586,7 @@
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>64</v>
@@ -3605,7 +3609,7 @@
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>64</v>
@@ -3628,7 +3632,7 @@
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>64</v>
@@ -3651,7 +3655,7 @@
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>64</v>
@@ -3674,7 +3678,7 @@
         <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>64</v>
@@ -3697,7 +3701,7 @@
         <v>7</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>64</v>
@@ -3720,7 +3724,7 @@
         <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>64</v>
@@ -3743,7 +3747,7 @@
         <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>64</v>
@@ -3766,7 +3770,7 @@
         <v>7</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>126</v>
+        <v>63</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>64</v>
@@ -3789,7 +3793,7 @@
         <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>64</v>
@@ -3812,7 +3816,7 @@
         <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>64</v>
@@ -3835,7 +3839,7 @@
         <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>64</v>
@@ -3858,7 +3862,7 @@
         <v>7</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>64</v>
@@ -3878,16 +3882,16 @@
         <v>30</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>122</v>
@@ -3901,16 +3905,16 @@
         <v>30</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>122</v>
@@ -3927,7 +3931,7 @@
         <v>6</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>66</v>
@@ -3950,7 +3954,7 @@
         <v>6</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>66</v>
@@ -3973,7 +3977,7 @@
         <v>6</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>66</v>
@@ -3996,7 +4000,7 @@
         <v>6</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>66</v>
@@ -4019,13 +4023,13 @@
         <v>6</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>122</v>
@@ -4042,13 +4046,13 @@
         <v>6</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>122</v>
@@ -4065,7 +4069,7 @@
         <v>6</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>12</v>
@@ -4088,7 +4092,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>12</v>
@@ -4111,7 +4115,7 @@
         <v>6</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>12</v>
@@ -4134,7 +4138,7 @@
         <v>6</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>12</v>
@@ -4157,7 +4161,7 @@
         <v>6</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>12</v>
@@ -4180,16 +4184,16 @@
         <v>6</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -4203,13 +4207,13 @@
         <v>6</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>122</v>
@@ -4226,16 +4230,16 @@
         <v>6</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -4249,7 +4253,7 @@
         <v>6</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -4269,16 +4273,16 @@
         <v>30</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>122</v>
@@ -4292,16 +4296,16 @@
         <v>30</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>122</v>
@@ -4318,7 +4322,7 @@
         <v>7</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>15</v>
@@ -4341,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>15</v>
@@ -4361,10 +4365,10 @@
         <v>30</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>15</v>
@@ -4372,8 +4376,8 @@
       <c r="F119" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G119" s="2" t="s">
-        <v>104</v>
+      <c r="G119" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -4387,7 +4391,7 @@
         <v>7</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>15</v>
@@ -4407,10 +4411,10 @@
         <v>30</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>15</v>
@@ -4418,8 +4422,8 @@
       <c r="F121" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G121" s="3" t="s">
-        <v>122</v>
+      <c r="G121" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4433,7 +4437,7 @@
         <v>7</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>15</v>
@@ -4456,7 +4460,7 @@
         <v>7</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>15</v>
@@ -4479,7 +4483,7 @@
         <v>7</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>15</v>
@@ -4502,7 +4506,7 @@
         <v>7</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>15</v>
@@ -4525,7 +4529,7 @@
         <v>7</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>15</v>
@@ -4548,7 +4552,7 @@
         <v>7</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>15</v>
@@ -4571,7 +4575,7 @@
         <v>7</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>15</v>
@@ -4594,7 +4598,7 @@
         <v>7</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>135</v>
+        <v>62</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>15</v>
@@ -4614,16 +4618,16 @@
         <v>30</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>122</v>
@@ -4637,16 +4641,16 @@
         <v>30</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>122</v>
@@ -4663,7 +4667,7 @@
         <v>6</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>16</v>
@@ -4686,7 +4690,7 @@
         <v>6</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>16</v>
@@ -4709,7 +4713,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>16</v>
@@ -4732,7 +4736,7 @@
         <v>6</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>16</v>
@@ -4755,7 +4759,7 @@
         <v>6</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>16</v>
@@ -4778,7 +4782,7 @@
         <v>6</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>16</v>
@@ -4801,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>16</v>
@@ -4824,7 +4828,7 @@
         <v>6</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>16</v>
@@ -4841,19 +4845,19 @@
         <v>29</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>122</v>
@@ -4864,19 +4868,19 @@
         <v>29</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>122</v>
@@ -4893,7 +4897,7 @@
         <v>7</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>36</v>
@@ -4916,7 +4920,7 @@
         <v>7</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>36</v>
@@ -4939,7 +4943,7 @@
         <v>7</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>36</v>
@@ -4962,7 +4966,7 @@
         <v>7</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>36</v>
@@ -4985,7 +4989,7 @@
         <v>7</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>36</v>
@@ -5008,7 +5012,7 @@
         <v>7</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>36</v>
@@ -5031,7 +5035,7 @@
         <v>7</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>36</v>
@@ -5054,7 +5058,7 @@
         <v>7</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>36</v>
@@ -5077,7 +5081,7 @@
         <v>7</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>36</v>
@@ -5100,7 +5104,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>36</v>
@@ -5123,7 +5127,7 @@
         <v>7</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>36</v>
@@ -5146,7 +5150,7 @@
         <v>7</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>36</v>
@@ -5169,13 +5173,13 @@
         <v>7</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>122</v>
@@ -5192,13 +5196,13 @@
         <v>7</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>122</v>
@@ -5215,13 +5219,13 @@
         <v>7</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>122</v>
@@ -5238,13 +5242,13 @@
         <v>7</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>122</v>
@@ -5258,19 +5262,19 @@
         <v>78</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -5284,7 +5288,7 @@
         <v>7</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>64</v>
@@ -5307,7 +5311,7 @@
         <v>6</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>64</v>
@@ -5330,7 +5334,7 @@
         <v>7</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>64</v>
@@ -5350,10 +5354,10 @@
         <v>78</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>64</v>
@@ -5361,8 +5365,8 @@
       <c r="F162" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G162" s="3" t="s">
-        <v>122</v>
+      <c r="G162" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -5376,7 +5380,7 @@
         <v>7</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>64</v>
@@ -5399,7 +5403,7 @@
         <v>7</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>64</v>
@@ -5422,7 +5426,7 @@
         <v>7</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>64</v>
@@ -5445,7 +5449,7 @@
         <v>7</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>64</v>
@@ -5468,7 +5472,7 @@
         <v>7</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>64</v>
@@ -5491,7 +5495,7 @@
         <v>7</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>64</v>
@@ -5514,7 +5518,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>64</v>
@@ -5537,7 +5541,7 @@
         <v>7</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>64</v>
@@ -5560,7 +5564,7 @@
         <v>7</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>64</v>
@@ -5583,7 +5587,7 @@
         <v>7</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>64</v>
@@ -5606,7 +5610,7 @@
         <v>7</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>64</v>
@@ -5629,7 +5633,7 @@
         <v>7</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>64</v>
@@ -5652,7 +5656,7 @@
         <v>7</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>64</v>
@@ -5675,7 +5679,7 @@
         <v>7</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>64</v>
@@ -5698,7 +5702,7 @@
         <v>7</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>64</v>
@@ -5721,7 +5725,7 @@
         <v>7</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>64</v>
@@ -5744,7 +5748,7 @@
         <v>7</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>64</v>
@@ -5767,7 +5771,7 @@
         <v>7</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>64</v>
@@ -5790,7 +5794,7 @@
         <v>7</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>64</v>
@@ -5813,7 +5817,7 @@
         <v>7</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>64</v>
@@ -5836,7 +5840,7 @@
         <v>7</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>64</v>
@@ -5859,7 +5863,7 @@
         <v>7</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>64</v>
@@ -5882,7 +5886,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>64</v>
@@ -5902,16 +5906,16 @@
         <v>78</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="G186" s="3" t="s">
         <v>122</v>
@@ -5925,22 +5929,22 @@
         <v>78</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>29</v>
       </c>
@@ -5951,16 +5955,16 @@
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>158</v>
+        <v>66</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G188" s="2" t="s">
-        <v>104</v>
+        <v>121</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -5974,16 +5978,16 @@
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G189" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -5994,19 +5998,19 @@
         <v>78</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G190" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -6020,16 +6024,16 @@
         <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G191" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -6043,16 +6047,16 @@
         <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G192" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
+      </c>
+      <c r="G192" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -6066,16 +6070,16 @@
         <v>7</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G193" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
+      </c>
+      <c r="G193" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -6086,16 +6090,16 @@
         <v>78</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G194" s="3" t="s">
         <v>122</v>
@@ -6109,16 +6113,16 @@
         <v>78</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G195" s="3" t="s">
         <v>122</v>
@@ -6135,7 +6139,7 @@
         <v>7</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>15</v>
@@ -6158,7 +6162,7 @@
         <v>7</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>15</v>
@@ -6181,7 +6185,7 @@
         <v>7</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>15</v>
@@ -6201,16 +6205,16 @@
         <v>78</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>122</v>
@@ -6224,16 +6228,16 @@
         <v>78</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G200" s="3" t="s">
         <v>122</v>
@@ -6247,16 +6251,16 @@
         <v>78</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>122</v>
@@ -6273,7 +6277,7 @@
         <v>6</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>16</v>
@@ -6285,8 +6289,78 @@
         <v>122</v>
       </c>
     </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>